<commit_message>
Update for 2020. Remove access to file of disaggregated GHG emissions.
</commit_message>
<xml_diff>
--- a/Data/Environmental_data/Minerals_extracted_in_Canada.xlsx
+++ b/Data/Environmental_data/Minerals_extracted_in_Canada.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Minerals_extension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Environmental_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB38347-16DB-430D-9ACF-514B78C980AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D5D022-0499-4430-A304-8E4E02279E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Allocate to lead/zinc extraction sectors</t>
   </si>
@@ -85,9 +96,6 @@
   </si>
   <si>
     <t>Lithium</t>
-  </si>
-  <si>
-    <t>Ore weight (spodumene) need to determine lithium content</t>
   </si>
   <si>
     <t>Mica</t>
@@ -604,19 +612,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="4">
         <v>2014</v>
@@ -633,11 +642,23 @@
       <c r="F1" s="4">
         <v>2018</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="4">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="4">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="4">
+        <v>2021</v>
+      </c>
+      <c r="J1" s="4">
+        <v>2022</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -654,36 +675,54 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="B4">
         <v>0</v>
       </c>
@@ -699,8 +738,20 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -719,10 +770,19 @@
       <c r="F5">
         <v>40000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>40000</v>
+      </c>
+      <c r="H5">
+        <v>50000</v>
+      </c>
+      <c r="I5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -739,8 +799,20 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -759,10 +831,19 @@
       <c r="F7">
         <v>600</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>600</v>
+      </c>
+      <c r="H7">
+        <v>650</v>
+      </c>
+      <c r="I7">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -779,8 +860,20 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -797,36 +890,60 @@
         <v>25</v>
       </c>
       <c r="F9">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="B11">
         <v>0</v>
       </c>
@@ -842,8 +959,20 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -860,12 +989,21 @@
         <v>1802</v>
       </c>
       <c r="F12">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1857</v>
+      </c>
+      <c r="G12">
+        <v>1803</v>
+      </c>
+      <c r="H12">
+        <v>1800</v>
+      </c>
+      <c r="I12">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -882,8 +1020,20 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -900,10 +1050,16 @@
         <v>6355</v>
       </c>
       <c r="F14">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6349</v>
+      </c>
+      <c r="G14">
+        <v>6075</v>
+      </c>
+      <c r="H14">
+        <v>5965</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -914,16 +1070,22 @@
         <v>715417</v>
       </c>
       <c r="D15">
-        <v>693059</v>
+        <v>695508</v>
       </c>
       <c r="E15">
-        <v>594994</v>
+        <v>597194</v>
       </c>
       <c r="F15">
-        <v>542900</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>542932</v>
+      </c>
+      <c r="G15">
+        <v>572705</v>
+      </c>
+      <c r="H15">
+        <v>584609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -942,34 +1104,52 @@
       <c r="F16">
         <v>23194</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <v>18638</v>
+      </c>
+      <c r="H16">
+        <v>13104</v>
+      </c>
+      <c r="K16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="B18">
         <v>0</v>
       </c>
@@ -985,8 +1165,20 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1003,12 +1195,15 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35000</v>
+      </c>
+      <c r="G19">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1025,8 +1220,20 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
@@ -1040,13 +1247,22 @@
         <v>161.49700000000001</v>
       </c>
       <c r="E21">
-        <v>168.072</v>
+        <v>172.87700000000001</v>
       </c>
       <c r="F21">
-        <v>183.047</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>191.88200000000001</v>
+      </c>
+      <c r="G21">
+        <v>190.65100000000001</v>
+      </c>
+      <c r="H21">
+        <v>178.05500000000001</v>
+      </c>
+      <c r="I21">
+        <v>222.524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1060,13 +1276,22 @@
         <v>35000</v>
       </c>
       <c r="E22">
-        <v>40000</v>
+        <v>14000</v>
       </c>
       <c r="F22">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11000</v>
+      </c>
+      <c r="G22">
+        <v>11000</v>
+      </c>
+      <c r="H22">
+        <v>11937</v>
+      </c>
+      <c r="I22">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1083,12 +1308,24 @@
         <v>3001000</v>
       </c>
       <c r="F23">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3240000</v>
+      </c>
+      <c r="G23">
+        <v>2408000</v>
+      </c>
+      <c r="H23">
+        <v>3050000</v>
+      </c>
+      <c r="I23">
+        <v>2400000</v>
+      </c>
+      <c r="J23">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1105,8 +1342,20 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
@@ -1123,12 +1372,24 @@
         <v>67</v>
       </c>
       <c r="F25">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="G25">
+        <v>64.8</v>
+      </c>
+      <c r="H25">
+        <v>60.6</v>
+      </c>
+      <c r="I25">
+        <v>44.3</v>
+      </c>
+      <c r="J25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1145,8 +1406,20 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -1163,10 +1436,22 @@
         <v>0.2</v>
       </c>
       <c r="F27">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.4</v>
+      </c>
+      <c r="G27">
+        <v>0.4</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1183,33 +1468,51 @@
         <v>30200000</v>
       </c>
       <c r="F28">
-        <v>31500000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31700000</v>
+      </c>
+      <c r="G28">
+        <v>35200000</v>
+      </c>
+      <c r="H28">
+        <v>36100000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="B30">
         <v>0</v>
       </c>
@@ -1225,8 +1528,20 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
@@ -1243,10 +1558,16 @@
         <v>13494</v>
       </c>
       <c r="F31">
-        <v>18947</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15605</v>
+      </c>
+      <c r="G31">
+        <v>21782</v>
+      </c>
+      <c r="H31">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>19</v>
       </c>
@@ -1263,75 +1584,111 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>114000</v>
-      </c>
-      <c r="G32" t="s">
+        <v>2433</v>
+      </c>
+      <c r="G32">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1343,15 +1700,24 @@
         <v>22000</v>
       </c>
       <c r="E36">
-        <v>24000</v>
+        <v>22000</v>
       </c>
       <c r="F36">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>21000</v>
+      </c>
+      <c r="G36">
+        <v>21000</v>
+      </c>
+      <c r="H36">
+        <v>15000</v>
+      </c>
+      <c r="I36">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37">
         <v>9358</v>
@@ -1366,12 +1732,21 @@
         <v>4765</v>
       </c>
       <c r="F37">
-        <v>4681</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5048</v>
+      </c>
+      <c r="G37">
+        <v>3896</v>
+      </c>
+      <c r="H37">
+        <v>2525</v>
+      </c>
+      <c r="I37">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38">
         <v>218223</v>
@@ -1386,12 +1761,15 @@
         <v>206354</v>
       </c>
       <c r="F38">
-        <v>175761</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>177867</v>
+      </c>
+      <c r="G38">
+        <v>181410</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39">
         <v>6000</v>
@@ -1403,15 +1781,24 @@
         <v>6300</v>
       </c>
       <c r="E39">
-        <v>7200</v>
+        <v>6981</v>
       </c>
       <c r="F39">
-        <v>7700</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7400</v>
+      </c>
+      <c r="G39">
+        <v>6600</v>
+      </c>
+      <c r="H39">
+        <v>6200</v>
+      </c>
+      <c r="I39">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40">
         <v>23</v>
@@ -1426,15 +1813,27 @@
         <v>19</v>
       </c>
       <c r="F40">
-        <v>20</v>
-      </c>
-      <c r="G40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40">
+        <v>21.9</v>
+      </c>
+      <c r="H40">
+        <v>10.9</v>
+      </c>
+      <c r="I40">
+        <v>15.4</v>
+      </c>
+      <c r="J40">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="K40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="B41">
         <v>1178000</v>
@@ -1449,55 +1848,85 @@
         <v>1459000</v>
       </c>
       <c r="F41">
-        <v>1240000</v>
-      </c>
-      <c r="G41" t="s">
+        <v>1306000</v>
+      </c>
+      <c r="G41">
+        <v>1259000</v>
+      </c>
+      <c r="H41">
+        <v>1400000</v>
+      </c>
+      <c r="K41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="B44">
         <v>7.2</v>
@@ -1512,15 +1941,27 @@
         <v>7.6</v>
       </c>
       <c r="F44">
-        <v>7.4</v>
-      </c>
-      <c r="G44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7.6</v>
+      </c>
+      <c r="G44">
+        <v>8.6</v>
+      </c>
+      <c r="H44">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>5.4</v>
+      </c>
+      <c r="K44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45">
         <v>11462000</v>
@@ -1535,33 +1976,54 @@
         <v>13835000</v>
       </c>
       <c r="F45">
-        <v>12270000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14024000</v>
+      </c>
+      <c r="G45">
+        <v>12770000</v>
+      </c>
+      <c r="H45">
+        <v>14239000</v>
+      </c>
+      <c r="I45">
+        <v>14593000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="B47">
         <v>0</v>
       </c>
@@ -1577,10 +2039,22 @@
       <c r="F47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>2011000</v>
@@ -1595,12 +2069,24 @@
         <v>2540000</v>
       </c>
       <c r="F48">
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4864000</v>
+      </c>
+      <c r="G48">
+        <v>4185000</v>
+      </c>
+      <c r="H48">
+        <v>4046000</v>
+      </c>
+      <c r="I48">
+        <v>4649000</v>
+      </c>
+      <c r="J48">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1617,10 +2103,22 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1637,10 +2135,22 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51">
         <v>0.6</v>
@@ -1655,12 +2165,24 @@
         <v>0.06</v>
       </c>
       <c r="F51">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+      <c r="G51">
+        <v>0.8</v>
+      </c>
+      <c r="H51">
+        <v>0.7</v>
+      </c>
+      <c r="I51">
+        <v>0.3</v>
+      </c>
+      <c r="J51">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B52">
         <v>0.2</v>
@@ -1675,12 +2197,24 @@
         <v>0.5</v>
       </c>
       <c r="F52">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+      <c r="G52">
+        <v>0.5</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53">
         <v>14473000</v>
@@ -1697,10 +2231,13 @@
       <c r="F53">
         <v>10713000</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>11936000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B54">
         <v>142</v>
@@ -1715,12 +2252,18 @@
         <v>72</v>
       </c>
       <c r="F54">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="G54">
+        <v>57</v>
+      </c>
+      <c r="H54">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B55">
         <v>472</v>
@@ -1732,15 +2275,24 @@
         <v>385</v>
       </c>
       <c r="E55">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F55">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+      <c r="G55">
+        <v>349.7</v>
+      </c>
+      <c r="H55">
+        <v>324.89999999999998</v>
+      </c>
+      <c r="I55">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1757,10 +2309,22 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57">
         <v>90000</v>
@@ -1775,12 +2339,21 @@
         <v>215000</v>
       </c>
       <c r="F57">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>279000</v>
+      </c>
+      <c r="G57">
+        <v>243000</v>
+      </c>
+      <c r="H57">
+        <v>153000</v>
+      </c>
+      <c r="I57">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -1797,10 +2370,22 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>8</v>
@@ -1815,12 +2400,18 @@
         <v>49</v>
       </c>
       <c r="F59">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G59">
+        <v>40</v>
+      </c>
+      <c r="H59">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1837,91 +2428,151 @@
       <c r="F60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="B65">
         <v>0</v>
       </c>
@@ -1937,30 +2588,42 @@
       <c r="F65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>10000</v>
+      </c>
+      <c r="F66">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>11000</v>
-      </c>
-      <c r="F66">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="B67">
         <v>322605</v>
@@ -1972,15 +2635,24 @@
         <v>301210</v>
       </c>
       <c r="E67">
-        <v>305314</v>
+        <v>305000</v>
       </c>
       <c r="F67">
-        <v>287119</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>305000</v>
+      </c>
+      <c r="G67">
+        <v>336000</v>
+      </c>
+      <c r="H67">
+        <v>248000</v>
+      </c>
+      <c r="I67">
+        <v>310000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -1997,9 +2669,21 @@
       <c r="F68">
         <v>0</v>
       </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G68">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K68">
     <sortCondition ref="A2:A68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>